<commit_message>
hub mega diag code started
</commit_message>
<xml_diff>
--- a/Docs/Pinout/Pinout Final.xlsx
+++ b/Docs/Pinout/Pinout Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Submarine-project\Docs\Pinout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WiderD\Documents\GitHub\Submarine-project\Docs\Pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4A2BAA-236B-4D89-A7AA-9437D327F2A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7043A1BB-084D-4C83-92CE-E8C04BAA5295}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3617116B-5A0D-4B79-B698-FBDD543C2C8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{3617116B-5A0D-4B79-B698-FBDD543C2C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Submarine Pinout</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>PARALLEL BUS - DIRECTION SENSE</t>
+  </si>
+  <si>
+    <t>Bonus PWM out of Front Bulkhead</t>
   </si>
 </sst>
 </file>
@@ -231,13 +234,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,65 +558,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE9BBE5-5DB6-43CD-9458-32EE2E67C973}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H3" t="s">
@@ -621,19 +625,19 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4">
@@ -647,19 +651,19 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5">
@@ -673,19 +677,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H6">
@@ -699,13 +703,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H7">
@@ -719,13 +723,13 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H8">
@@ -733,13 +737,13 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H9">
@@ -747,13 +751,13 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H10">
@@ -761,13 +765,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H11">
@@ -775,31 +779,39 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+    </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17">
@@ -810,7 +822,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B18">
@@ -821,7 +833,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19">
@@ -832,7 +844,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B20">
@@ -843,7 +855,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B21">
@@ -854,7 +866,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22">
@@ -865,17 +877,17 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B25">
@@ -886,7 +898,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B26">
@@ -897,7 +909,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B27">
@@ -909,13 +921,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A16:F16"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
spool and ribbon cable stuff
</commit_message>
<xml_diff>
--- a/Docs/Pinout/Pinout Final.xlsx
+++ b/Docs/Pinout/Pinout Final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Submarine-project\Docs\Pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4A2BAA-236B-4D89-A7AA-9437D327F2A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20254A3-E778-4711-B129-FDE3E13B9B74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3617116B-5A0D-4B79-B698-FBDD543C2C8D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Submarine Pinout</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>PARALLEL BUS - DIRECTION SENSE</t>
+  </si>
+  <si>
+    <t>Bonus PWM to front</t>
   </si>
 </sst>
 </file>
@@ -231,13 +234,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,65 +558,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE9BBE5-5DB6-43CD-9458-32EE2E67C973}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H3" t="s">
@@ -621,19 +624,19 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4">
@@ -647,19 +650,19 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5">
@@ -673,19 +676,19 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H6">
@@ -699,13 +702,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H7">
@@ -719,13 +722,13 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H8">
@@ -733,13 +736,13 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H9">
@@ -747,13 +750,13 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H10">
@@ -761,13 +764,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H11">
@@ -775,31 +778,39 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
     </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+    </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17">
@@ -810,7 +821,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B18">
@@ -821,7 +832,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19">
@@ -832,7 +843,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B20">
@@ -843,7 +854,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B21">
@@ -854,7 +865,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22">
@@ -865,17 +876,17 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B25">
@@ -886,7 +897,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B26">
@@ -897,7 +908,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B27">
@@ -909,13 +920,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J2:L2"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A16:F16"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>